<commit_message>
plots and more data tidying
</commit_message>
<xml_diff>
--- a/input/qe_prog_data.xlsx
+++ b/input/qe_prog_data.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harryaustin/R/Dissertation/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43EE236A-32DC-B049-9B4C-4DC9CCB0C103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F93F85-CB1E-BB42-A3A8-C7C2163D51F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="16260" activeTab="2" xr2:uid="{B5F025EF-521A-664C-8962-A17373687D47}"/>
+    <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="16260" activeTab="1" xr2:uid="{B5F025EF-521A-664C-8962-A17373687D47}"/>
   </bookViews>
   <sheets>
     <sheet name="programme" sheetId="2" r:id="rId1"/>
-    <sheet name="maturity_sectors" sheetId="3" r:id="rId2"/>
-    <sheet name="maturity_sectors_2" sheetId="4" r:id="rId3"/>
+    <sheet name="announcements" sheetId="5" r:id="rId2"/>
+    <sheet name="maturity_sectors" sheetId="3" r:id="rId3"/>
+    <sheet name="maturity_sectors_2" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029" iterateDelta="252"/>
+  <calcPr calcId="191029" iterateDelta="252"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="36">
   <si>
     <t>QE5</t>
   </si>
@@ -107,6 +108,45 @@
   </si>
   <si>
     <t>def_range</t>
+  </si>
+  <si>
+    <t>announcement</t>
+  </si>
+  <si>
+    <t>QE1a</t>
+  </si>
+  <si>
+    <t>QE1b</t>
+  </si>
+  <si>
+    <t>QE1c</t>
+  </si>
+  <si>
+    <t>QE1d</t>
+  </si>
+  <si>
+    <t>QE2a</t>
+  </si>
+  <si>
+    <t>QE2b</t>
+  </si>
+  <si>
+    <t>QE3a</t>
+  </si>
+  <si>
+    <t>QE4a</t>
+  </si>
+  <si>
+    <t>QE5a</t>
+  </si>
+  <si>
+    <t>QE5b</t>
+  </si>
+  <si>
+    <t>QE5c</t>
+  </si>
+  <si>
+    <t>announcement_date</t>
   </si>
 </sst>
 </file>
@@ -124,6 +164,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -152,13 +193,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,7 +528,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection sqref="A1:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -559,6 +610,160 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B96382D9-E51A-5743-85D8-20329F913E03}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="2">
+        <v>39877</v>
+      </c>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="8"/>
+      <c r="B3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="2">
+        <v>39940</v>
+      </c>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="8"/>
+      <c r="B4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="2">
+        <v>40031</v>
+      </c>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="8"/>
+      <c r="B5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="2">
+        <v>40122</v>
+      </c>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="2">
+        <v>40822</v>
+      </c>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="7"/>
+      <c r="B7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="2">
+        <v>40948</v>
+      </c>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="2">
+        <v>41095</v>
+      </c>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="2">
+        <v>42586</v>
+      </c>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="2">
+        <v>43909</v>
+      </c>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="7"/>
+      <c r="B11" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="2">
+        <v>44000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="7"/>
+      <c r="B12" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="2">
+        <v>44140</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A2:A5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A67FB921-BB04-CD4A-B2E9-673DE43A04BB}">
   <dimension ref="A1:H5"/>
   <sheetViews>
@@ -585,24 +790,24 @@
       <c r="C1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="5">
+      <c r="A2" s="4">
         <v>39883</v>
       </c>
       <c r="B2" t="s">
@@ -623,12 +828,12 @@
       <c r="G2">
         <v>25</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2" s="4">
         <v>40031</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="5">
+      <c r="A3" s="4">
         <v>40031</v>
       </c>
       <c r="B3">
@@ -649,12 +854,12 @@
       <c r="G3" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="4">
         <v>40948</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="5">
+      <c r="A4" s="4">
         <v>40948</v>
       </c>
       <c r="B4">
@@ -675,12 +880,12 @@
       <c r="G4" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="4">
         <v>43899</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>43899</v>
       </c>
       <c r="B5">
@@ -701,7 +906,7 @@
       <c r="G5" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="4">
         <v>44545</v>
       </c>
     </row>
@@ -710,18 +915,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5917C62-68B1-7145-92DA-5A66417B5E9B}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -738,7 +943,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="5">
+      <c r="A2" s="4">
         <v>40031</v>
       </c>
       <c r="B2" t="s">
@@ -755,7 +960,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="5">
+      <c r="A3" s="4">
         <v>40948</v>
       </c>
       <c r="B3">
@@ -772,7 +977,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="5">
+      <c r="A4" s="4">
         <v>43899</v>
       </c>
       <c r="B4">
@@ -789,7 +994,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>44545</v>
       </c>
       <c r="B5">
@@ -806,7 +1011,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>40031</v>
       </c>
       <c r="B6">
@@ -823,7 +1028,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="5">
+      <c r="A7" s="4">
         <v>40948</v>
       </c>
       <c r="B7">
@@ -840,7 +1045,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="5">
+      <c r="A8" s="4">
         <v>43899</v>
       </c>
       <c r="B8">
@@ -857,7 +1062,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="5">
+      <c r="A9" s="4">
         <v>44545</v>
       </c>
       <c r="B9">
@@ -874,7 +1079,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="5">
+      <c r="A10" s="4">
         <v>40031</v>
       </c>
       <c r="B10">
@@ -891,7 +1096,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="5">
+      <c r="A11" s="4">
         <v>40948</v>
       </c>
       <c r="B11">
@@ -908,7 +1113,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="5">
+      <c r="A12" s="4">
         <v>43899</v>
       </c>
       <c r="B12">
@@ -925,7 +1130,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="5">
+      <c r="A13" s="4">
         <v>44545</v>
       </c>
       <c r="B13">

</xml_diff>